<commit_message>
finish the supervised learning part
</commit_message>
<xml_diff>
--- a/07_Project_Capstone_Arvato-Bertelsmann/data/concept.xlsx
+++ b/07_Project_Capstone_Arvato-Bertelsmann/data/concept.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://trw1-my.sharepoint.com/personal/robin_wesselmann_zf_com/Documents/Desktop/Udacity_DataScientist_Class/07_Project_Capstone_Arvato-Bertelsmann/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\z635177\OneDrive - ZF Friedrichshafen AG\Desktop\Udacity_DataScientist_Class\07_Project_Capstone_Arvato-Bertelsmann\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{723A4C71-F861-443F-9357-F2DAB68EE4DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E4343AB-A4DA-4481-9F85-23D684469A56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{525E5AD0-F98D-4885-A96B-0DC5D28A960A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{525E5AD0-F98D-4885-A96B-0DC5D28A960A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="CUSTOMER_SEGMENTATION" sheetId="1" r:id="rId1"/>
+    <sheet name="SUPERVISED_LEARNING" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,14 +36,24 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF4EC9B0"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -65,8 +76,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -75,6 +89,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF3333FF"/>
+      <color rgb="FF65F117"/>
       <color rgb="FF000000"/>
       <color rgb="FFFF8F8F"/>
     </mruColors>
@@ -2078,6 +2094,4663 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>447674</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>476249</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="33" name="Rechteck: abgerundete Ecken 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F593D9CD-80A0-6D1B-72D5-EE5954846113}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1285874" y="2047875"/>
+          <a:ext cx="2543175" cy="495300"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent4">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100" b="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Udacity_MAILOUT_052018_TRAIN.csv</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>809625</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="35" name="Rechteck: abgerundete Ecken 34">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1CA5FAA3-B0BD-B82B-BF14-AA0BD7588E61}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4162425" y="1752600"/>
+          <a:ext cx="1514475" cy="438150"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="3333FF"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>X_train</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>819150</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>657225</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="36" name="Rechteck: abgerundete Ecken 35">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F28DAF81-449E-4676-9DAF-5E393D58F428}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4171950" y="2419350"/>
+          <a:ext cx="1514475" cy="438150"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="3333FF"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>y_train</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>295276</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>657225</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="38" name="Rechteck: abgerundete Ecken 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{12933E12-3F90-47A6-9DC1-ED3392FB5678}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6162676" y="1714500"/>
+          <a:ext cx="1200149" cy="504825"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1000">
+              <a:solidFill>
+                <a:srgbClr val="3333FF"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Replace</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1000" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="3333FF"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> unknown values</a:t>
+          </a:r>
+          <a:endParaRPr lang="de-DE" sz="1000">
+            <a:solidFill>
+              <a:srgbClr val="3333FF"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>295276</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>657225</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="40" name="Rechteck: abgerundete Ecken 39">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8BBED4D7-D973-48B2-8762-BE7A03660C38}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6162676" y="2447925"/>
+          <a:ext cx="1200149" cy="504825"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1000">
+              <a:solidFill>
+                <a:srgbClr val="3333FF"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Drop specific</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1000" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="3333FF"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> columns</a:t>
+          </a:r>
+          <a:endParaRPr lang="de-DE" sz="1000">
+            <a:solidFill>
+              <a:srgbClr val="3333FF"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>38101</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="41" name="Rechteck: abgerundete Ecken 40">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A466E98C-CE8A-47F0-87B5-FEEA5CE78AFC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7581901" y="1704975"/>
+          <a:ext cx="1200149" cy="504825"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1000">
+              <a:solidFill>
+                <a:srgbClr val="3333FF"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Handle</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1000" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="3333FF"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> missing columns</a:t>
+          </a:r>
+          <a:endParaRPr lang="de-DE" sz="1000">
+            <a:solidFill>
+              <a:srgbClr val="3333FF"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>38101</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="42" name="Rechteck: abgerundete Ecken 41">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8959B0CB-FEF8-4988-A521-03DFDC69B735}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7581901" y="2428875"/>
+          <a:ext cx="1200149" cy="504825"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1000">
+              <a:solidFill>
+                <a:srgbClr val="3333FF"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Handle high</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1000" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="3333FF"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> correlation</a:t>
+          </a:r>
+          <a:endParaRPr lang="de-DE" sz="1000">
+            <a:solidFill>
+              <a:srgbClr val="3333FF"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>619126</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="43" name="Rechteck: abgerundete Ecken 42">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C54B9FC9-EE0D-4A75-A46F-F73A7EB67F96}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9001126" y="1704975"/>
+          <a:ext cx="1200149" cy="504825"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1000">
+              <a:solidFill>
+                <a:srgbClr val="3333FF"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Process youth years</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>619126</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="44" name="Rechteck: abgerundete Ecken 43">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C18E9632-51F3-4E91-A276-0BDC8356F669}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9001126" y="2419350"/>
+          <a:ext cx="1200149" cy="504825"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1000">
+              <a:solidFill>
+                <a:srgbClr val="3333FF"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Impute</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1000" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="3333FF"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> missing data</a:t>
+          </a:r>
+          <a:endParaRPr lang="de-DE" sz="1000">
+            <a:solidFill>
+              <a:srgbClr val="3333FF"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>352426</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>714375</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="45" name="Rechteck: abgerundete Ecken 44">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8105F9B9-A921-49B5-B7C5-9BE5640BCFB9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10410826" y="1704975"/>
+          <a:ext cx="1200149" cy="504825"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1000">
+              <a:solidFill>
+                <a:srgbClr val="3333FF"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Encode</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1000" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="3333FF"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> Features</a:t>
+          </a:r>
+          <a:endParaRPr lang="de-DE" sz="1000">
+            <a:solidFill>
+              <a:srgbClr val="3333FF"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>352426</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>714375</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="46" name="Rechteck: abgerundete Ecken 45">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{14EDE192-E081-48DA-B720-D93EEBDEA5B9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10410826" y="2409825"/>
+          <a:ext cx="1200149" cy="504825"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1000">
+              <a:solidFill>
+                <a:srgbClr val="3333FF"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Scaling Features</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>556354</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>80562</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="47" name="Rechteck: abgerundete Ecken 46">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E418F3DC-882F-419E-A492-F20097DD5ED5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13122468" y="2067384"/>
+          <a:ext cx="1199690" cy="512743"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1000">
+              <a:solidFill>
+                <a:srgbClr val="3333FF"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>ML</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1000" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="3333FF"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> Model</a:t>
+          </a:r>
+          <a:endParaRPr lang="de-DE" sz="1000">
+            <a:solidFill>
+              <a:srgbClr val="3333FF"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>714375</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>172139</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="48" name="Rechteck 47">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{117C2F06-A741-E78D-0B4C-5ECD534F7C76}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4065339" y="1621316"/>
+          <a:ext cx="10348396" cy="1449865"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="dash"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>657225</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2683299" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="49" name="Textfeld 48">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{64EB5DD7-07A1-9195-754E-4169B7300FAF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4010025" y="1333500"/>
+          <a:ext cx="2683299" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Preprocessing</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100" baseline="0"/>
+            <a:t> / ML Crossvalidation Pipeline</a:t>
+          </a:r>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>57151</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>57151</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="51" name="Gerade Verbindung mit Pfeil 50">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{64A70897-1816-0283-B271-1AE4AF6AD751}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="38" idx="2"/>
+          <a:endCxn id="40" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6762751" y="2219325"/>
+          <a:ext cx="0" cy="228600"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>657225</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>147638</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>38101</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>166688</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="53" name="Verbinder: gewinkelt 52">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E0FA1989-5686-21FC-4D25-42FB41893BA5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="40" idx="3"/>
+          <a:endCxn id="41" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="7362825" y="1957388"/>
+          <a:ext cx="219076" cy="742950"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>147638</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>619126</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>147638</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="54" name="Verbinder: gewinkelt 53">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F53A8135-320D-40AE-916A-C5A8D4AC1E61}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="42" idx="3"/>
+          <a:endCxn id="43" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="8782050" y="1957388"/>
+          <a:ext cx="219076" cy="723900"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>147638</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>352426</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>138113</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="57" name="Verbinder: gewinkelt 56">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6697ABE9-53EC-4F40-BE84-BF69ADAE9420}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="44" idx="3"/>
+          <a:endCxn id="45" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="10201275" y="1957388"/>
+          <a:ext cx="209551" cy="714375"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>638176</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>638176</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="60" name="Gerade Verbindung mit Pfeil 59">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D872C6B9-05E7-456F-8B46-370836DEDBCC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="41" idx="2"/>
+          <a:endCxn id="42" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8181976" y="2209800"/>
+          <a:ext cx="0" cy="219075"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>381001</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>381001</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="63" name="Gerade Verbindung mit Pfeil 62">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2510B32D-EA9A-470A-8D13-464BA2FB8043}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="43" idx="2"/>
+          <a:endCxn id="44" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9601201" y="2209800"/>
+          <a:ext cx="0" cy="209550"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>114301</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>114301</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="66" name="Gerade Verbindung mit Pfeil 65">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{224FF1F4-AD14-45BB-BE4F-96287BC8B708}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="45" idx="2"/>
+          <a:endCxn id="46" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11010901" y="2209800"/>
+          <a:ext cx="0" cy="200025"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>657225</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>157163</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>295276</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="72" name="Verbinder: gewinkelt 71">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C04133A-EE53-46E9-AAB4-5A54ECFD3C84}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="36" idx="3"/>
+          <a:endCxn id="38" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5686425" y="1966913"/>
+          <a:ext cx="476251" cy="671512"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>157163</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>295276</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="75" name="Gerade Verbindung mit Pfeil 74">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{37FEE580-901C-4D08-914B-29A576C916A6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="35" idx="3"/>
+          <a:endCxn id="38" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5676900" y="1966913"/>
+          <a:ext cx="485776" cy="4762"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>634390</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>653440</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="78" name="Rechteck 77">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1579C60-2925-431F-613E-557D295892FC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14875986" y="1931395"/>
+          <a:ext cx="1694532" cy="822822"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+          <a:prstTxWarp prst="textNoShape">
+            <a:avLst/>
+          </a:prstTxWarp>
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:endParaRPr lang="de-DE" sz="1000">
+            <a:solidFill>
+              <a:srgbClr val="3333FF"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>172139</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>139433</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>634390</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>142876</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="80" name="Gerade Verbindung mit Pfeil 79">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{514F5F8D-E3D9-264E-C2F0-CDB0853EF719}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="48" idx="3"/>
+          <a:endCxn id="78" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="14413735" y="2342806"/>
+          <a:ext cx="462251" cy="3443"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>476249</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>809625</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="81" name="Verbinder: gewinkelt 80">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC8F18AA-8F84-4CBF-AC8C-EB51756F38CA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="33" idx="3"/>
+          <a:endCxn id="35" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3829049" y="1971675"/>
+          <a:ext cx="333376" cy="323850"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>476249</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>819150</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="84" name="Verbinder: gewinkelt 83">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1110622-71AB-4336-94D0-A23AD73563ED}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="33" idx="3"/>
+          <a:endCxn id="36" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3829049" y="2295525"/>
+          <a:ext cx="342901" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>558190</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="619080" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="87" name="Textfeld 86">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3AAD268-788B-4623-BC37-157E07FCC090}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14799786" y="1681105"/>
+          <a:ext cx="619080" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Metrics</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>604425</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>80550</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="88" name="Ellipse 87">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0E70EFE-6594-CC56-CD0F-D7E713FE345A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1190625" y="1276350"/>
+          <a:ext cx="252000" cy="252000"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFF00"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>1</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>371474</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>400049</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="89" name="Rechteck: abgerundete Ecken 88">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{611C1B62-3F6F-401D-8E34-99C01D87C796}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1209674" y="4152900"/>
+          <a:ext cx="2543175" cy="495300"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent4">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100" b="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Udacity_MAILOUT_052018_TRAIN.csv</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>733425</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="90" name="Rechteck: abgerundete Ecken 89">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C1A7845-FDC9-482E-BA62-569FD401194C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4086225" y="3857625"/>
+          <a:ext cx="1514475" cy="438150"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="3333FF"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>X_train</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>742950</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="91" name="Rechteck: abgerundete Ecken 90">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42E08C44-4570-4E9B-A435-A8A4DF572B1A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4095750" y="4524375"/>
+          <a:ext cx="1514475" cy="438150"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="3333FF"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>y_train</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>219076</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="92" name="Rechteck: abgerundete Ecken 91">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0CF0F233-41E7-4DB0-8A8F-C6573EBEFEAF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6086476" y="3819525"/>
+          <a:ext cx="1200149" cy="504825"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1000">
+              <a:solidFill>
+                <a:srgbClr val="3333FF"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Replace</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1000" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="3333FF"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> unknown values</a:t>
+          </a:r>
+          <a:endParaRPr lang="de-DE" sz="1000">
+            <a:solidFill>
+              <a:srgbClr val="3333FF"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>219076</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="93" name="Rechteck: abgerundete Ecken 92">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EA181D9F-A5D0-4FB0-AA7A-12FBA6C1E030}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6086476" y="4552950"/>
+          <a:ext cx="1200149" cy="504825"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1000">
+              <a:solidFill>
+                <a:srgbClr val="3333FF"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Drop specific</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1000" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="3333FF"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> columns</a:t>
+          </a:r>
+          <a:endParaRPr lang="de-DE" sz="1000">
+            <a:solidFill>
+              <a:srgbClr val="3333FF"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>800101</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="94" name="Rechteck: abgerundete Ecken 93">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FAF90897-B5A6-474F-B9E9-38E6B8FE7317}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7505701" y="3810000"/>
+          <a:ext cx="1200149" cy="504825"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1000">
+              <a:solidFill>
+                <a:srgbClr val="3333FF"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Handle</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1000" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="3333FF"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> missing columns</a:t>
+          </a:r>
+          <a:endParaRPr lang="de-DE" sz="1000">
+            <a:solidFill>
+              <a:srgbClr val="3333FF"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>800101</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="95" name="Rechteck: abgerundete Ecken 94">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{16737FEF-EC2F-4E5D-8D79-FF48E9680856}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7505701" y="4533900"/>
+          <a:ext cx="1200149" cy="504825"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1000">
+              <a:solidFill>
+                <a:srgbClr val="3333FF"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Handle high</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1000" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="3333FF"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> correlation</a:t>
+          </a:r>
+          <a:endParaRPr lang="de-DE" sz="1000">
+            <a:solidFill>
+              <a:srgbClr val="3333FF"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>542926</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="96" name="Rechteck: abgerundete Ecken 95">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3BA720A-B639-4559-A7B5-C1AABDA6C0F2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8924926" y="3810000"/>
+          <a:ext cx="1200149" cy="504825"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1000">
+              <a:solidFill>
+                <a:srgbClr val="3333FF"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Process youth years</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>542926</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="97" name="Rechteck: abgerundete Ecken 96">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4D776407-576C-47A8-A382-96A1A8450720}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8924926" y="4524375"/>
+          <a:ext cx="1200149" cy="504825"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1000">
+              <a:solidFill>
+                <a:srgbClr val="3333FF"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Impute</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1000" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="3333FF"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> missing data</a:t>
+          </a:r>
+          <a:endParaRPr lang="de-DE" sz="1000">
+            <a:solidFill>
+              <a:srgbClr val="3333FF"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>276226</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>638175</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="98" name="Rechteck: abgerundete Ecken 97">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41E1E62A-12AE-4E5A-B13D-B7E74CFAE33A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10334626" y="3810000"/>
+          <a:ext cx="1200149" cy="504825"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1000">
+              <a:solidFill>
+                <a:srgbClr val="3333FF"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Encode</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1000" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="3333FF"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> Features</a:t>
+          </a:r>
+          <a:endParaRPr lang="de-DE" sz="1000">
+            <a:solidFill>
+              <a:srgbClr val="3333FF"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>276226</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>638175</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="99" name="Rechteck: abgerundete Ecken 98">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A04FE50F-6FDE-4718-860E-C2FC900F240B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10334626" y="4514850"/>
+          <a:ext cx="1200149" cy="504825"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1000">
+              <a:solidFill>
+                <a:srgbClr val="3333FF"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Scaling Features</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>556354</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>166171</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>80562</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>128071</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="100" name="Rechteck: abgerundete Ecken 99">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{24517AED-AB9B-4D4E-ABC8-C949939BAD85}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13122468" y="4205689"/>
+          <a:ext cx="1199690" cy="512743"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1000">
+              <a:solidFill>
+                <a:srgbClr val="3333FF"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>ML</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1000" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="3333FF"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> Model</a:t>
+          </a:r>
+          <a:endParaRPr lang="de-DE" sz="1000">
+            <a:solidFill>
+              <a:srgbClr val="3333FF"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>638175</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>183615</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="101" name="Rechteck 100">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2DFBD94B-EAB1-4C54-8949-B03855241178}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3989139" y="3758014"/>
+          <a:ext cx="10436072" cy="1449866"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="dash"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3561809" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="102" name="Textfeld 101">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5E0B88C-C8D9-4126-855D-34CC732A7319}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3933825" y="3438525"/>
+          <a:ext cx="3561809" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Preprocessing</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100" baseline="0"/>
+            <a:t> / ML Pipeline </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100" b="1" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="3333FF"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>(Crossvalidation + Gridsearch)</a:t>
+          </a:r>
+          <a:endParaRPr lang="de-DE" sz="1100" b="1">
+            <a:solidFill>
+              <a:srgbClr val="3333FF"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>819151</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>819151</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="103" name="Gerade Verbindung mit Pfeil 102">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29AD0A08-EAE4-4F97-B210-32C82AB2AD21}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="92" idx="2"/>
+          <a:endCxn id="93" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6686551" y="4324350"/>
+          <a:ext cx="0" cy="228600"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>80963</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>800101</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>100013</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="104" name="Verbinder: gewinkelt 103">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C8FAEDE9-469F-4FA5-BD52-5F1BAE0460E8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="93" idx="3"/>
+          <a:endCxn id="94" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="7286625" y="4062413"/>
+          <a:ext cx="219076" cy="742950"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>80963</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>542926</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>80963</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="105" name="Verbinder: gewinkelt 104">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{666CDB43-1751-46D3-A870-34AAAE501E18}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="95" idx="3"/>
+          <a:endCxn id="96" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="8705850" y="4062413"/>
+          <a:ext cx="219076" cy="723900"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>80963</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>276226</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>71438</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="106" name="Verbinder: gewinkelt 105">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{423853F9-57AD-4EB6-B643-170BECB1B7BF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="97" idx="3"/>
+          <a:endCxn id="98" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="10125075" y="4062413"/>
+          <a:ext cx="209551" cy="714375"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>561976</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>561976</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="107" name="Gerade Verbindung mit Pfeil 106">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D2BFFC07-3B3D-4C71-AD73-07EF1AC54C8E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="94" idx="2"/>
+          <a:endCxn id="95" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8105776" y="4314825"/>
+          <a:ext cx="0" cy="219075"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>304801</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>304801</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="108" name="Gerade Verbindung mit Pfeil 107">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{701D57DA-8739-45FB-8E33-34FBD3C7086A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="96" idx="2"/>
+          <a:endCxn id="97" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9525001" y="4314825"/>
+          <a:ext cx="0" cy="209550"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>38101</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>38101</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="109" name="Gerade Verbindung mit Pfeil 108">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B7CBF74A-8BB5-49F9-BAFD-4251C83AFDA7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="98" idx="2"/>
+          <a:endCxn id="99" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10934701" y="4314825"/>
+          <a:ext cx="0" cy="200025"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>90488</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>219076</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="111" name="Verbinder: gewinkelt 110">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A06937C-09FC-40DE-9485-F80B3EECE6D8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="91" idx="3"/>
+          <a:endCxn id="92" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5610225" y="4071938"/>
+          <a:ext cx="476251" cy="671512"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>90488</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>219076</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="112" name="Gerade Verbindung mit Pfeil 111">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D7AF08E7-4101-4F54-8934-F8231CFC58D4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="90" idx="3"/>
+          <a:endCxn id="92" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5600700" y="4071938"/>
+          <a:ext cx="485776" cy="4762"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>558190</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>577240</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="113" name="Rechteck 112">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{430920E4-F5EB-4946-9C20-DE79696C6206}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14799786" y="4068093"/>
+          <a:ext cx="1694532" cy="820183"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+          <a:prstTxWarp prst="textNoShape">
+            <a:avLst/>
+          </a:prstTxWarp>
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:endParaRPr lang="de-DE" sz="1000">
+            <a:solidFill>
+              <a:srgbClr val="3333FF"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>183615</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>71438</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>558190</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="114" name="Gerade Verbindung mit Pfeil 113">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99473A53-1DEF-4DF8-A658-B1E74E9BDC1F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="101" idx="3"/>
+          <a:endCxn id="113" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="14425211" y="4478185"/>
+          <a:ext cx="374575" cy="4762"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>400049</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>733425</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="115" name="Verbinder: gewinkelt 114">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{40ED1781-65BA-43E9-BD6F-08B239355845}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="89" idx="3"/>
+          <a:endCxn id="90" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3752849" y="4076700"/>
+          <a:ext cx="333376" cy="323850"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>400049</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>742950</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="116" name="Verbinder: gewinkelt 115">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{906BDD75-E591-48CE-ACC1-9A1173286AA8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="89" idx="3"/>
+          <a:endCxn id="91" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3752849" y="4400550"/>
+          <a:ext cx="342901" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>481990</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="922240" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="117" name="Textfeld 116">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{24E3B433-DD4E-47F5-A049-4EF653A76AA8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14723586" y="3815164"/>
+          <a:ext cx="922240" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Final Metrics</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>528225</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>13875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="118" name="Ellipse 117">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D37F0D43-49EF-4729-BA2A-285989A79BD4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1114425" y="3381375"/>
+          <a:ext cx="252000" cy="252000"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFF00"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>2</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>88823</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>221714</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="119" name="Rechteck: abgerundete Ecken 118">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F880D8C1-7B9C-6B73-9EF8-F99C5A4A8D3F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16843642" y="1747780"/>
+          <a:ext cx="970632" cy="1082637"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="65F117">
+            <a:alpha val="27843"/>
+          </a:srgbClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="3333FF"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Choice of model</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>529615</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>187174</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>151257</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="120" name="Pfeil: nach rechts 119">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4A1A5F7-3D53-1AF1-501C-AEE725DD9716}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16446693" y="2048334"/>
+          <a:ext cx="495300" cy="489911"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>580915</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1126847" cy="578885"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="121" name="Textfeld 120">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54C29546-2B98-41E2-8919-279F6D75DFB5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13147029" y="560368"/>
+          <a:ext cx="1126847" cy="578885"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="ctr">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Multiple Models</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>in For Loop</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>306598</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>37566</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>318458</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="123" name="Gerade Verbindung mit Pfeil 122">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{313C8544-975F-C405-48B3-4295363D2AF4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="121" idx="2"/>
+          <a:endCxn id="47" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13710453" y="1139253"/>
+          <a:ext cx="11860" cy="928131"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>318458</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>574139</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>166172</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="125" name="Verbinder: gewinkelt 124">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B6234A22-D37A-45B4-A010-3894526B8413}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="119" idx="2"/>
+          <a:endCxn id="100" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="14838000" y="1714731"/>
+          <a:ext cx="1375272" cy="3606645"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>38216</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>40969</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>400165</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>2869</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rechteck: abgerundete Ecken 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB946F98-E38E-482D-909C-6BAD81992A15}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11766589" y="2060728"/>
+          <a:ext cx="1199690" cy="512743"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1000">
+              <a:solidFill>
+                <a:srgbClr val="3333FF"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Random</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1000">
+              <a:solidFill>
+                <a:srgbClr val="3333FF"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Undersampling</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>714375</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>2869</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>638061</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>129908</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Verbinder: gewinkelt 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C49181F7-4B46-4CCA-8387-47CF8F1289B0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="46" idx="3"/>
+          <a:endCxn id="4" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="11605008" y="2573471"/>
+          <a:ext cx="761426" cy="127039"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>400165</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>113727</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>556354</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>120383</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="Gerade Verbindung mit Pfeil 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4EE78D7C-24CD-4958-B5B1-D355308B16C8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="4" idx="3"/>
+          <a:endCxn id="47" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12966279" y="2317100"/>
+          <a:ext cx="156189" cy="6656"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>38216</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>166171</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>400165</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>128071</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Rechteck: abgerundete Ecken 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3EE49810-878E-4D73-9424-3D5C19D3B98E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11766589" y="4205689"/>
+          <a:ext cx="1199690" cy="512743"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1000">
+              <a:solidFill>
+                <a:srgbClr val="3333FF"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Random</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1000">
+              <a:solidFill>
+                <a:srgbClr val="3333FF"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Undersampling</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>638175</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>128071</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>638061</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>60593</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="12" name="Verbinder: gewinkelt 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{24F03156-0333-497C-BCD2-A93B38E4E2B7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="99" idx="3"/>
+          <a:endCxn id="11" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="11528808" y="4718432"/>
+          <a:ext cx="837626" cy="116137"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>400165</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>55314</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>556354</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>55314</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="15" name="Gerade Verbindung mit Pfeil 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20D7C676-A3CD-4EC8-B35F-BBA8B0D59E4A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="11" idx="3"/>
+          <a:endCxn id="100" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12966279" y="4462061"/>
+          <a:ext cx="156189" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2380,7 +7053,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E88715E-8548-4B53-AF75-46E96E452561}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
@@ -2389,4 +7062,23 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA1610DD-F345-4072-B07D-F1FC8168FBD7}">
+  <dimension ref="H32"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="83" workbookViewId="0">
+      <selection activeCell="J35" sqref="J35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="32" spans="8:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="H32" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>